<commit_message>
Calculo de tiempo terminado
</commit_message>
<xml_diff>
--- a/archivos/Calculo de tiempo.xlsx
+++ b/archivos/Calculo de tiempo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>Proyecto:</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Lenguaje</t>
   </si>
   <si>
-    <t>NodeJS</t>
-  </si>
-  <si>
     <t>Modulo</t>
   </si>
   <si>
@@ -79,13 +76,112 @@
   </si>
   <si>
     <t>Inventario de  EPP's</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Creacion de ordenes</t>
+  </si>
+  <si>
+    <t>Correctivo puntual</t>
+  </si>
+  <si>
+    <t>Correctivo x Garantia</t>
+  </si>
+  <si>
+    <t>Creacion Correctivos</t>
+  </si>
+  <si>
+    <t>Creacion Preventivo</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Proyecto</t>
+  </si>
+  <si>
+    <t>Odenes</t>
+  </si>
+  <si>
+    <t>Calendario</t>
+  </si>
+  <si>
+    <t>Mensajes</t>
+  </si>
+  <si>
+    <t>TIEMPO</t>
+  </si>
+  <si>
+    <t>1 DIA</t>
+  </si>
+  <si>
+    <t>(CONFIRMAR CON CHRISTIAN)</t>
+  </si>
+  <si>
+    <t>2 DIAS</t>
+  </si>
+  <si>
+    <t>(CONFIRMAR CON VERO Y CHRISTIAN)</t>
+  </si>
+  <si>
+    <t>3 DIAS</t>
+  </si>
+  <si>
+    <t>2DIAS</t>
+  </si>
+  <si>
+    <t>CANCELADO</t>
+  </si>
+  <si>
+    <t>4 DIAS</t>
+  </si>
+  <si>
+    <t>Creacion de calendarios</t>
+  </si>
+  <si>
+    <t>Creacion de preventivos (CRUD)</t>
+  </si>
+  <si>
+    <t>Lista de mensajes</t>
+  </si>
+  <si>
+    <t>Crear+enviar mensaje</t>
+  </si>
+  <si>
+    <t>Obtener mensajes</t>
+  </si>
+  <si>
+    <t>Responder mensajes</t>
+  </si>
+  <si>
+    <t>Notificaciones instantaneas</t>
+  </si>
+  <si>
+    <t>Creacion de orden</t>
+  </si>
+  <si>
+    <t>Mensaje recibido</t>
+  </si>
+  <si>
+    <t>Evento del calendario</t>
+  </si>
+  <si>
+    <t>5 DIAS</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +189,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,8 +229,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -170,15 +298,22 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -186,21 +321,60 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,148 +656,549 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E22"/>
+  <dimension ref="A3:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <f>_xlfn.NUMBERVALUE(IF(D8&lt;&gt;"",MID(D8,1,1),0))</f>
+        <v>1</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <f t="shared" ref="A9:A44" si="0">_xlfn.NUMBERVALUE(IF(D9&lt;&gt;"",MID(D9,1,1),0))</f>
+        <v>2</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="13"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
+        <v>0</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="C26" s="10"/>
+      <c r="D26" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="14"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+      <c r="C28" s="3"/>
+      <c r="D28" s="14"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="5"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="14"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="21">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="8"/>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="21">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="10"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="21">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="10"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="10"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="21">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" t="s">
+        <v>34</v>
+      </c>
+      <c r="H44" s="17"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C45" s="16"/>
+      <c r="D45" s="19" t="str">
+        <f>CONCATENATE(SUM(A8:A44)," ","DIAS")</f>
+        <v>58 DIAS</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
+  <mergeCells count="40">
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D26:D29"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>